<commit_message>
New Version with unpivot pivot Data
New Version with unpivot pivot Data
</commit_message>
<xml_diff>
--- a/PivotData.xlsx
+++ b/PivotData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Transfer Jun-2023\Amit Files\Google Drive\Kanerika\power bi\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8049859-4A77-480A-A063-524D1193C733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7416D1DA-04A3-4641-8828-BA4A39450B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="12" xr2:uid="{267C35E5-4570-4798-B7F2-E927E6025BAC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="14" xr2:uid="{267C35E5-4570-4798-B7F2-E927E6025BAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="Fill" sheetId="7" r:id="rId12"/>
     <sheet name="Month on Col" sheetId="14" r:id="rId13"/>
     <sheet name="Product" sheetId="12" r:id="rId14"/>
+    <sheet name="Unpivot Pivot" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6993" uniqueCount="1824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7034" uniqueCount="1864">
   <si>
     <t>Name</t>
   </si>
@@ -5518,6 +5519,126 @@
   </si>
   <si>
     <t>A10</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>I4</t>
+  </si>
+  <si>
+    <t>I5</t>
+  </si>
+  <si>
+    <t>State 1</t>
+  </si>
+  <si>
+    <t>Value 1</t>
+  </si>
+  <si>
+    <t>State 2</t>
+  </si>
+  <si>
+    <t>Value 2</t>
+  </si>
+  <si>
+    <t>State 3</t>
+  </si>
+  <si>
+    <t>Value 3</t>
+  </si>
+  <si>
+    <t>State 4</t>
+  </si>
+  <si>
+    <t>Value 4</t>
+  </si>
+  <si>
+    <t>State 5</t>
+  </si>
+  <si>
+    <t>Value 5</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>S8</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>S19</t>
+  </si>
+  <si>
+    <t>S20</t>
+  </si>
+  <si>
+    <t>S21</t>
+  </si>
+  <si>
+    <t>S22</t>
+  </si>
+  <si>
+    <t>S23</t>
+  </si>
+  <si>
+    <t>S24</t>
+  </si>
+  <si>
+    <t>S25</t>
   </si>
 </sst>
 </file>
@@ -6493,7 +6614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DBA21F-C90E-45F2-B04B-206DA9273D7F}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7:G11"/>
     </sheetView>
   </sheetViews>
@@ -30551,6 +30672,232 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8645F09-9064-4D2E-9BDC-934E046BF4EB}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1831</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1832</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1833</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1834</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1836</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1837</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1844</v>
+      </c>
+      <c r="E2">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1849</v>
+      </c>
+      <c r="G2">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1854</v>
+      </c>
+      <c r="I2">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1859</v>
+      </c>
+      <c r="K2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1840</v>
+      </c>
+      <c r="C3">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1845</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1850</v>
+      </c>
+      <c r="G3">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1855</v>
+      </c>
+      <c r="I3">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1860</v>
+      </c>
+      <c r="K3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C4">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1846</v>
+      </c>
+      <c r="E4">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1851</v>
+      </c>
+      <c r="G4">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1856</v>
+      </c>
+      <c r="I4">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1861</v>
+      </c>
+      <c r="K4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1842</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1847</v>
+      </c>
+      <c r="E5">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1852</v>
+      </c>
+      <c r="G5">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1857</v>
+      </c>
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5" t="s">
+        <v>1862</v>
+      </c>
+      <c r="K5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1848</v>
+      </c>
+      <c r="E6">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1853</v>
+      </c>
+      <c r="G6">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1858</v>
+      </c>
+      <c r="I6">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1863</v>
+      </c>
+      <c r="K6">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F541E5-3554-4099-8326-D6393EE7A7E7}">
   <dimension ref="A1:C26"/>

</xml_diff>